<commit_message>
add DC and AN
</commit_message>
<xml_diff>
--- a/data/master_course_info.xlsx
+++ b/data/master_course_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3d893debe0afcb60/Desktop/Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC10487699DE4F865BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43972CAE-5389-4F37-8270-8C7EEE1F29B1}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_F25DC773A252ABDACC10487699DE4F865BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C21A046-7D88-42EA-91E5-F544073BC4F0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
   <si>
     <t>Abbre.</t>
   </si>
@@ -179,6 +179,21 @@
   </si>
   <si>
     <t>Prof. Omakar Sahoo</t>
+  </si>
+  <si>
+    <t>7MP501NE22</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>Art of Negotiation</t>
+  </si>
+  <si>
+    <t>Prof. Nitin Pillai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prof. Sapan Oza (VF) </t>
   </si>
 </sst>
 </file>
@@ -203,6 +218,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -301,7 +317,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,9 +344,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -626,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -752,10 +765,10 @@
       <c r="D6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -775,7 +788,7 @@
       <c r="E7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -792,10 +805,10 @@
       <c r="D8" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -812,10 +825,10 @@
       <c r="D9" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -829,7 +842,7 @@
       <c r="C10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>49</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -846,13 +859,13 @@
       <c r="C11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>50</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -891,6 +904,43 @@
         <v>13</v>
       </c>
       <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>